<commit_message>
adding litter and trash visuals
</commit_message>
<xml_diff>
--- a/NYCHA_outcomes.xlsx
+++ b/NYCHA_outcomes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ariadna/Box Sync/Ariadna/NYCHA_visualizations/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C1993726-14FC-3349-B8DE-717134103B67}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E679CD44-CD7D-F64F-A184-5D9111A99982}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12200" yWindow="460" windowWidth="15620" windowHeight="16580" activeTab="1" xr2:uid="{92086B50-FE46-B64C-9F5E-EE236EC2145E}"/>
+    <workbookView xWindow="16620" yWindow="460" windowWidth="15620" windowHeight="16580" activeTab="1" xr2:uid="{92086B50-FE46-B64C-9F5E-EE236EC2145E}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -836,10 +836,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{77359DB0-FF41-7D48-8AA5-53296189C0CC}">
-  <dimension ref="A1:A35"/>
+  <dimension ref="A1:B35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:A1048576"/>
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -847,122 +847,138 @@
     <col min="1" max="1" width="28.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1">
+    <row r="1" spans="1:2">
       <c r="A1" s="3" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="3" spans="1:1">
+    <row r="3" spans="1:2">
       <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:1">
+    <row r="4" spans="1:2">
       <c r="A4" s="2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:1">
+    <row r="5" spans="1:2">
       <c r="A5" s="2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:1">
+    <row r="6" spans="1:2">
       <c r="A6" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="8" spans="1:1">
+      <c r="B6">
+        <f>208.1-171.1</f>
+        <v>37</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
       <c r="A8" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:1">
+    <row r="9" spans="1:2">
       <c r="A9" s="1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="10" spans="1:1">
+      <c r="B9">
+        <f>143.3-183</f>
+        <v>-39.699999999999989</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2">
       <c r="A10" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="11" spans="1:1">
+    <row r="11" spans="1:2">
       <c r="A11" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="13" spans="1:1">
+    <row r="13" spans="1:2">
       <c r="A13" s="3" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="15" spans="1:1">
+    <row r="15" spans="1:2">
       <c r="A15" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:1">
+    <row r="16" spans="1:2">
       <c r="A16" s="2" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="17" spans="1:1">
+      <c r="B16">
+        <f>63.7-50.5</f>
+        <v>13.200000000000003</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2">
       <c r="A17" s="2" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="18" spans="1:1">
+    <row r="18" spans="1:2">
       <c r="A18" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="20" spans="1:1">
+    <row r="20" spans="1:2">
       <c r="A20" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="21" spans="1:1">
+    <row r="21" spans="1:2">
       <c r="A21" s="2" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="22" spans="1:1">
+      <c r="B21">
+        <f>41.3-48.2</f>
+        <v>-6.9000000000000057</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2">
       <c r="A22" s="2" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="23" spans="1:1">
+    <row r="23" spans="1:2">
       <c r="A23" s="1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="25" spans="1:1">
+    <row r="25" spans="1:2">
       <c r="A25" s="3" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="27" spans="1:1">
+    <row r="27" spans="1:2">
       <c r="A27" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:1">
+    <row r="28" spans="1:2">
       <c r="A28" s="2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="29" spans="1:1">
+    <row r="29" spans="1:2">
       <c r="A29" s="2" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="30" spans="1:1">
+    <row r="30" spans="1:2">
       <c r="A30" s="1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="32" spans="1:1">
+    <row r="32" spans="1:2">
       <c r="A32" s="1" t="s">
         <v>4</v>
       </c>

</xml_diff>

<commit_message>
edits to gifs and extrapolations graph
</commit_message>
<xml_diff>
--- a/NYCHA_outcomes.xlsx
+++ b/NYCHA_outcomes.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ariadna/Box Sync/Ariadna/NYCHA_visualizations/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E679CD44-CD7D-F64F-A184-5D9111A99982}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5405BF95-88E3-CC49-A600-E7A35CB8E439}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="16620" yWindow="460" windowWidth="15620" windowHeight="16580" activeTab="1" xr2:uid="{92086B50-FE46-B64C-9F5E-EE236EC2145E}"/>
+    <workbookView xWindow="16620" yWindow="460" windowWidth="15620" windowHeight="16580" activeTab="2" xr2:uid="{92086B50-FE46-B64C-9F5E-EE236EC2145E}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
     <sheet name="Hoja2" sheetId="2" r:id="rId2"/>
+    <sheet name="extrapolations" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -32,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="44">
   <si>
     <t>Control Group</t>
   </si>
@@ -227,6 +228,39 @@
   </si>
   <si>
     <t xml:space="preserve">Treatment </t>
+  </si>
+  <si>
+    <t>weight</t>
+  </si>
+  <si>
+    <t>1.5 car engines</t>
+  </si>
+  <si>
+    <t>1 Toyota</t>
+  </si>
+  <si>
+    <t>5 Hummers</t>
+  </si>
+  <si>
+    <t>equivalence</t>
+  </si>
+  <si>
+    <t>time_period</t>
+  </si>
+  <si>
+    <t>4 car tires</t>
+  </si>
+  <si>
+    <t>1 week</t>
+  </si>
+  <si>
+    <t>1 month</t>
+  </si>
+  <si>
+    <t>1 day</t>
+  </si>
+  <si>
+    <t>1 year</t>
   </si>
 </sst>
 </file>
@@ -838,8 +872,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{77359DB0-FF41-7D48-8AA5-53296189C0CC}">
   <dimension ref="A1:B35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -1001,4 +1035,74 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F06A7A90-910E-5546-8D19-108E98702448}">
+  <dimension ref="A1:C5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2">
+        <v>80</v>
+      </c>
+      <c r="B2" t="s">
+        <v>42</v>
+      </c>
+      <c r="C2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3">
+        <v>560</v>
+      </c>
+      <c r="B3" t="s">
+        <v>40</v>
+      </c>
+      <c r="C3" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4">
+        <v>2240</v>
+      </c>
+      <c r="B4" t="s">
+        <v>41</v>
+      </c>
+      <c r="C4" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5">
+        <v>26880</v>
+      </c>
+      <c r="B5" t="s">
+        <v>43</v>
+      </c>
+      <c r="C5" t="s">
+        <v>36</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>